<commit_message>
study: update ex41-2 file
</commit_message>
<xml_diff>
--- a/mysql/220801_ex41_2.xlsx
+++ b/mysql/220801_ex41_2.xlsx
@@ -5,17 +5,17 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\user\Desktop\github\SeSAC4_web\mysql\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\juok\00SW\GitHub\SeSAC4_web\mysql\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C16FA6A3-1C2E-427B-A80F-B8B18298A54C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1615B548-4876-403B-9027-C780A1E71C6B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1882" yWindow="338" windowWidth="20198" windowHeight="15472" activeTab="2" xr2:uid="{3CEB5B6F-1D00-4C3B-A773-D50126FCAA23}"/>
+    <workbookView xWindow="11628" yWindow="36" windowWidth="11376" windowHeight="11520" firstSheet="2" activeTab="2" xr2:uid="{3CEB5B6F-1D00-4C3B-A773-D50126FCAA23}"/>
   </bookViews>
   <sheets>
     <sheet name="user_table " sheetId="3" r:id="rId1"/>
     <sheet name="product_table" sheetId="4" r:id="rId2"/>
-    <sheet name="order_table" sheetId="5" r:id="rId3"/>
+    <sheet name="ordered_table" sheetId="5" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -45,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="160" uniqueCount="75">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="160" uniqueCount="76">
   <si>
     <t>No</t>
     <phoneticPr fontId="2" type="noConversion"/>
@@ -293,10 +293,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>order</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
     <t>주문 정보</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -381,11 +377,19 @@
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t>date</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
     <t>N</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>datetime</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>"FREE"</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ordered</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
@@ -602,36 +606,15 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="7" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -662,6 +645,30 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="7" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -979,465 +986,465 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9D3659E9-95AB-4052-B556-74648B2124AC}">
   <dimension ref="A2:J25"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="N11" sqref="N11"/>
+    <sheetView topLeftCell="F1" workbookViewId="0">
+      <selection activeCell="G21" sqref="G21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16.899999999999999"/>
+  <sheetFormatPr defaultRowHeight="17.399999999999999"/>
   <cols>
-    <col min="1" max="1" width="13.1875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.25" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15.3125" customWidth="1"/>
-    <col min="4" max="4" width="15.25" customWidth="1"/>
+    <col min="1" max="1" width="13.19921875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.19921875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.296875" customWidth="1"/>
+    <col min="4" max="4" width="15.19921875" customWidth="1"/>
     <col min="5" max="5" width="11" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="9.4375" customWidth="1"/>
-    <col min="7" max="7" width="6.875" customWidth="1"/>
-    <col min="8" max="8" width="6.125" customWidth="1"/>
-    <col min="9" max="9" width="5.8125" customWidth="1"/>
-    <col min="10" max="10" width="9.8125" customWidth="1"/>
+    <col min="6" max="6" width="9.3984375" customWidth="1"/>
+    <col min="7" max="7" width="6.8984375" customWidth="1"/>
+    <col min="8" max="8" width="6.09765625" customWidth="1"/>
+    <col min="9" max="9" width="5.796875" customWidth="1"/>
+    <col min="10" max="10" width="9.796875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:10" ht="16.899999999999999" customHeight="1">
+    <row r="2" spans="1:10" ht="16.95" customHeight="1">
       <c r="A2" s="1"/>
-      <c r="B2" s="4" t="s">
+      <c r="B2" s="15" t="s">
         <v>36</v>
       </c>
-      <c r="C2" s="5"/>
-      <c r="D2" s="6" t="s">
+      <c r="C2" s="16"/>
+      <c r="D2" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="E2" s="4" t="s">
+      <c r="E2" s="15" t="s">
         <v>37</v>
       </c>
-      <c r="F2" s="5"/>
-      <c r="G2" s="7" t="s">
+      <c r="F2" s="16"/>
+      <c r="G2" s="17" t="s">
         <v>5</v>
       </c>
-      <c r="H2" s="8"/>
-      <c r="I2" s="8"/>
-      <c r="J2" s="9"/>
+      <c r="H2" s="18"/>
+      <c r="I2" s="18"/>
+      <c r="J2" s="19"/>
     </row>
     <row r="3" spans="1:10">
       <c r="A3" s="1"/>
-      <c r="B3" s="4" t="s">
+      <c r="B3" s="15" t="s">
         <v>6</v>
       </c>
-      <c r="C3" s="5"/>
-      <c r="D3" s="7" t="s">
+      <c r="C3" s="16"/>
+      <c r="D3" s="17" t="s">
         <v>42</v>
       </c>
-      <c r="E3" s="8"/>
-      <c r="F3" s="8"/>
-      <c r="G3" s="8"/>
-      <c r="H3" s="8"/>
-      <c r="I3" s="8"/>
-      <c r="J3" s="9"/>
-    </row>
-    <row r="4" spans="1:10" ht="17.25" thickBot="1">
+      <c r="E3" s="18"/>
+      <c r="F3" s="18"/>
+      <c r="G3" s="18"/>
+      <c r="H3" s="18"/>
+      <c r="I3" s="18"/>
+      <c r="J3" s="19"/>
+    </row>
+    <row r="4" spans="1:10" ht="18" thickBot="1">
       <c r="A4" s="1"/>
-      <c r="B4" s="10" t="s">
+      <c r="B4" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="C4" s="11" t="s">
+      <c r="C4" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="D4" s="12" t="s">
+      <c r="D4" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="E4" s="10" t="s">
+      <c r="E4" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="F4" s="10" t="s">
+      <c r="F4" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="G4" s="10" t="s">
+      <c r="G4" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="H4" s="10" t="s">
+      <c r="H4" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="I4" s="10" t="s">
+      <c r="I4" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="J4" s="10" t="s">
+      <c r="J4" s="3" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="5" spans="1:10">
       <c r="A5" s="1"/>
-      <c r="B5" s="13">
+      <c r="B5" s="6">
         <v>1</v>
       </c>
-      <c r="C5" s="14" t="s">
+      <c r="C5" s="7" t="s">
         <v>28</v>
       </c>
-      <c r="D5" s="15" t="s">
+      <c r="D5" s="8" t="s">
         <v>29</v>
       </c>
-      <c r="E5" s="16" t="s">
+      <c r="E5" s="9" t="s">
         <v>19</v>
       </c>
-      <c r="F5" s="13">
+      <c r="F5" s="6">
         <v>15</v>
       </c>
-      <c r="G5" s="13" t="s">
+      <c r="G5" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="H5" s="13" t="s">
+      <c r="H5" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="I5" s="13"/>
-      <c r="J5" s="13" t="s">
+      <c r="I5" s="6"/>
+      <c r="J5" s="6" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="6" spans="1:10">
       <c r="A6" s="1"/>
-      <c r="B6" s="13">
+      <c r="B6" s="6">
         <v>2</v>
       </c>
-      <c r="C6" s="14" t="s">
+      <c r="C6" s="7" t="s">
         <v>30</v>
       </c>
-      <c r="D6" s="15" t="s">
+      <c r="D6" s="8" t="s">
         <v>31</v>
       </c>
-      <c r="E6" s="14" t="s">
+      <c r="E6" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="F6" s="17">
+      <c r="F6" s="10">
         <v>10</v>
       </c>
-      <c r="G6" s="13" t="s">
+      <c r="G6" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="H6" s="13"/>
-      <c r="I6" s="17"/>
-      <c r="J6" s="13" t="s">
+      <c r="H6" s="6"/>
+      <c r="I6" s="10"/>
+      <c r="J6" s="6" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="7" spans="1:10">
       <c r="A7" s="1"/>
-      <c r="B7" s="13">
+      <c r="B7" s="6">
         <v>3</v>
       </c>
-      <c r="C7" s="14" t="s">
-        <v>69</v>
-      </c>
-      <c r="D7" s="15" t="s">
+      <c r="C7" s="7" t="s">
+        <v>68</v>
+      </c>
+      <c r="D7" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="E7" s="14" t="s">
+      <c r="E7" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="F7" s="17">
+      <c r="F7" s="10">
         <v>20</v>
       </c>
-      <c r="G7" s="13" t="s">
+      <c r="G7" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="H7" s="13"/>
-      <c r="I7" s="17"/>
-      <c r="J7" s="13" t="s">
+      <c r="H7" s="6"/>
+      <c r="I7" s="10"/>
+      <c r="J7" s="6" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="8" spans="1:10">
       <c r="A8" s="1"/>
-      <c r="B8" s="13">
+      <c r="B8" s="6">
         <v>4</v>
       </c>
-      <c r="C8" s="14" t="s">
-        <v>70</v>
-      </c>
-      <c r="D8" s="15" t="s">
+      <c r="C8" s="7" t="s">
+        <v>69</v>
+      </c>
+      <c r="D8" s="8" t="s">
         <v>21</v>
       </c>
-      <c r="E8" s="14" t="s">
+      <c r="E8" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="F8" s="17">
+      <c r="F8" s="10">
         <v>30</v>
       </c>
-      <c r="G8" s="13" t="s">
+      <c r="G8" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="H8" s="13"/>
-      <c r="I8" s="17"/>
-      <c r="J8" s="13" t="s">
+      <c r="H8" s="6"/>
+      <c r="I8" s="10"/>
+      <c r="J8" s="6" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="9" spans="1:10">
       <c r="A9" s="1"/>
-      <c r="B9" s="13">
+      <c r="B9" s="6">
         <v>5</v>
       </c>
-      <c r="C9" s="14" t="s">
-        <v>71</v>
-      </c>
-      <c r="D9" s="15" t="s">
+      <c r="C9" s="7" t="s">
+        <v>70</v>
+      </c>
+      <c r="D9" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="E9" s="14" t="s">
+      <c r="E9" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="F9" s="17">
+      <c r="F9" s="10">
         <v>15</v>
       </c>
-      <c r="G9" s="13" t="s">
+      <c r="G9" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="H9" s="17"/>
-      <c r="I9" s="17"/>
-      <c r="J9" s="13" t="s">
+      <c r="H9" s="10"/>
+      <c r="I9" s="10"/>
+      <c r="J9" s="6" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="10" spans="1:10">
       <c r="A10" s="1"/>
-      <c r="B10" s="13">
+      <c r="B10" s="6">
         <v>6</v>
       </c>
-      <c r="C10" s="14" t="s">
+      <c r="C10" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="D10" s="15" t="s">
+      <c r="D10" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="E10" s="14" t="s">
+      <c r="E10" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="F10" s="17">
+      <c r="F10" s="10">
         <v>2</v>
       </c>
-      <c r="G10" s="13" t="s">
+      <c r="G10" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="H10" s="17"/>
-      <c r="I10" s="17"/>
-      <c r="J10" s="18" t="s">
+      <c r="H10" s="10"/>
+      <c r="I10" s="10"/>
+      <c r="J10" s="11" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="11" spans="1:10">
       <c r="A11" s="1"/>
-      <c r="B11" s="13">
+      <c r="B11" s="6">
         <v>7</v>
       </c>
-      <c r="C11" s="14" t="s">
+      <c r="C11" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="D11" s="15" t="s">
+      <c r="D11" s="8" t="s">
         <v>24</v>
       </c>
-      <c r="E11" s="14" t="s">
+      <c r="E11" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="F11" s="17"/>
-      <c r="G11" s="13" t="s">
-        <v>16</v>
-      </c>
-      <c r="H11" s="17"/>
-      <c r="I11" s="17"/>
-      <c r="J11" s="13" t="s">
+      <c r="F11" s="10"/>
+      <c r="G11" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="H11" s="10"/>
+      <c r="I11" s="10"/>
+      <c r="J11" s="6" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="12" spans="1:10">
       <c r="A12" s="1"/>
-      <c r="B12" s="13">
+      <c r="B12" s="6">
         <v>8</v>
       </c>
-      <c r="C12" s="14" t="s">
-        <v>64</v>
-      </c>
-      <c r="D12" s="14" t="s">
+      <c r="C12" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="D12" s="7" t="s">
         <v>47</v>
       </c>
-      <c r="E12" s="14" t="s">
+      <c r="E12" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="F12" s="17">
+      <c r="F12" s="10">
         <v>50</v>
       </c>
-      <c r="G12" s="13" t="s">
-        <v>16</v>
-      </c>
-      <c r="H12" s="17"/>
-      <c r="I12" s="17"/>
-      <c r="J12" s="13" t="s">
-        <v>18</v>
+      <c r="G12" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="H12" s="10"/>
+      <c r="I12" s="10"/>
+      <c r="J12" s="20" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="13" spans="1:10">
       <c r="A13" s="1"/>
-      <c r="B13" s="13">
+      <c r="B13" s="6">
         <v>9</v>
       </c>
-      <c r="C13" s="14" t="s">
-        <v>56</v>
-      </c>
-      <c r="D13" s="14" t="s">
+      <c r="C13" s="7" t="s">
+        <v>55</v>
+      </c>
+      <c r="D13" s="7" t="s">
+        <v>71</v>
+      </c>
+      <c r="E13" s="7" t="s">
+        <v>73</v>
+      </c>
+      <c r="F13" s="10"/>
+      <c r="G13" s="6" t="s">
         <v>72</v>
       </c>
-      <c r="E13" s="14" t="s">
-        <v>73</v>
-      </c>
-      <c r="F13" s="17"/>
-      <c r="G13" s="13" t="s">
-        <v>74</v>
-      </c>
-      <c r="H13" s="17"/>
-      <c r="I13" s="17"/>
-      <c r="J13" s="13" t="s">
+      <c r="H13" s="10"/>
+      <c r="I13" s="10"/>
+      <c r="J13" s="6" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="14" spans="1:10">
       <c r="A14" s="1"/>
-      <c r="B14" s="13"/>
-      <c r="C14" s="14"/>
-      <c r="D14" s="14"/>
-      <c r="E14" s="14"/>
-      <c r="F14" s="17"/>
-      <c r="G14" s="13"/>
-      <c r="H14" s="17"/>
-      <c r="I14" s="17"/>
-      <c r="J14" s="17"/>
+      <c r="B14" s="6"/>
+      <c r="C14" s="7"/>
+      <c r="D14" s="7"/>
+      <c r="E14" s="7"/>
+      <c r="F14" s="10"/>
+      <c r="G14" s="6"/>
+      <c r="H14" s="10"/>
+      <c r="I14" s="10"/>
+      <c r="J14" s="10"/>
     </row>
     <row r="15" spans="1:10">
       <c r="A15" s="1"/>
-      <c r="B15" s="13"/>
-      <c r="C15" s="14"/>
-      <c r="D15" s="14"/>
-      <c r="E15" s="14"/>
-      <c r="F15" s="17"/>
-      <c r="G15" s="13"/>
-      <c r="H15" s="17"/>
-      <c r="I15" s="17"/>
-      <c r="J15" s="17"/>
+      <c r="B15" s="6"/>
+      <c r="C15" s="7"/>
+      <c r="D15" s="7"/>
+      <c r="E15" s="7"/>
+      <c r="F15" s="10"/>
+      <c r="G15" s="6"/>
+      <c r="H15" s="10"/>
+      <c r="I15" s="10"/>
+      <c r="J15" s="10"/>
     </row>
     <row r="16" spans="1:10">
       <c r="A16" s="1"/>
-      <c r="B16" s="13"/>
-      <c r="C16" s="14"/>
-      <c r="D16" s="14"/>
-      <c r="E16" s="14"/>
-      <c r="F16" s="17"/>
-      <c r="G16" s="13"/>
-      <c r="H16" s="17"/>
-      <c r="I16" s="17"/>
-      <c r="J16" s="17"/>
+      <c r="B16" s="6"/>
+      <c r="C16" s="7"/>
+      <c r="D16" s="7"/>
+      <c r="E16" s="7"/>
+      <c r="F16" s="10"/>
+      <c r="G16" s="6"/>
+      <c r="H16" s="10"/>
+      <c r="I16" s="10"/>
+      <c r="J16" s="10"/>
     </row>
     <row r="17" spans="1:10">
       <c r="A17" s="1"/>
-      <c r="B17" s="13"/>
-      <c r="C17" s="14"/>
-      <c r="D17" s="14"/>
-      <c r="E17" s="14"/>
-      <c r="F17" s="17"/>
-      <c r="G17" s="13"/>
-      <c r="H17" s="17"/>
-      <c r="I17" s="17"/>
-      <c r="J17" s="17"/>
+      <c r="B17" s="6"/>
+      <c r="C17" s="7"/>
+      <c r="D17" s="7"/>
+      <c r="E17" s="7"/>
+      <c r="F17" s="10"/>
+      <c r="G17" s="6"/>
+      <c r="H17" s="10"/>
+      <c r="I17" s="10"/>
+      <c r="J17" s="10"/>
     </row>
     <row r="18" spans="1:10">
       <c r="A18" s="1"/>
-      <c r="B18" s="13"/>
-      <c r="C18" s="14"/>
-      <c r="D18" s="14"/>
-      <c r="E18" s="14"/>
-      <c r="F18" s="17"/>
-      <c r="G18" s="13"/>
-      <c r="H18" s="17"/>
-      <c r="I18" s="17"/>
-      <c r="J18" s="17"/>
+      <c r="B18" s="6"/>
+      <c r="C18" s="7"/>
+      <c r="D18" s="7"/>
+      <c r="E18" s="7"/>
+      <c r="F18" s="10"/>
+      <c r="G18" s="6"/>
+      <c r="H18" s="10"/>
+      <c r="I18" s="10"/>
+      <c r="J18" s="10"/>
     </row>
     <row r="19" spans="1:10">
       <c r="A19" s="1"/>
-      <c r="B19" s="13"/>
-      <c r="C19" s="14"/>
-      <c r="D19" s="14"/>
-      <c r="E19" s="14"/>
-      <c r="F19" s="17"/>
-      <c r="G19" s="13"/>
-      <c r="H19" s="17"/>
-      <c r="I19" s="17"/>
-      <c r="J19" s="17"/>
+      <c r="B19" s="6"/>
+      <c r="C19" s="7"/>
+      <c r="D19" s="7"/>
+      <c r="E19" s="7"/>
+      <c r="F19" s="10"/>
+      <c r="G19" s="6"/>
+      <c r="H19" s="10"/>
+      <c r="I19" s="10"/>
+      <c r="J19" s="10"/>
     </row>
     <row r="20" spans="1:10">
       <c r="A20" s="1"/>
-      <c r="B20" s="13"/>
-      <c r="C20" s="14"/>
-      <c r="D20" s="14"/>
-      <c r="E20" s="14"/>
-      <c r="F20" s="17"/>
-      <c r="G20" s="13"/>
-      <c r="H20" s="17"/>
-      <c r="I20" s="17"/>
-      <c r="J20" s="17"/>
+      <c r="B20" s="6"/>
+      <c r="C20" s="7"/>
+      <c r="D20" s="7"/>
+      <c r="E20" s="7"/>
+      <c r="F20" s="10"/>
+      <c r="G20" s="6"/>
+      <c r="H20" s="10"/>
+      <c r="I20" s="10"/>
+      <c r="J20" s="10"/>
     </row>
     <row r="21" spans="1:10">
       <c r="A21" s="1"/>
-      <c r="B21" s="13"/>
-      <c r="C21" s="14"/>
-      <c r="D21" s="14"/>
-      <c r="E21" s="14"/>
-      <c r="F21" s="17"/>
-      <c r="G21" s="13"/>
-      <c r="H21" s="17"/>
-      <c r="I21" s="17"/>
-      <c r="J21" s="17"/>
+      <c r="B21" s="6"/>
+      <c r="C21" s="7"/>
+      <c r="D21" s="7"/>
+      <c r="E21" s="7"/>
+      <c r="F21" s="10"/>
+      <c r="G21" s="6"/>
+      <c r="H21" s="10"/>
+      <c r="I21" s="10"/>
+      <c r="J21" s="10"/>
     </row>
     <row r="22" spans="1:10">
       <c r="A22" s="1"/>
-      <c r="B22" s="13"/>
-      <c r="C22" s="14"/>
-      <c r="D22" s="14"/>
-      <c r="E22" s="14"/>
-      <c r="F22" s="17"/>
-      <c r="G22" s="13"/>
-      <c r="H22" s="17"/>
-      <c r="I22" s="17"/>
-      <c r="J22" s="17"/>
+      <c r="B22" s="6"/>
+      <c r="C22" s="7"/>
+      <c r="D22" s="7"/>
+      <c r="E22" s="7"/>
+      <c r="F22" s="10"/>
+      <c r="G22" s="6"/>
+      <c r="H22" s="10"/>
+      <c r="I22" s="10"/>
+      <c r="J22" s="10"/>
     </row>
     <row r="23" spans="1:10">
       <c r="A23" s="1"/>
-      <c r="B23" s="17"/>
-      <c r="C23" s="14"/>
-      <c r="D23" s="14"/>
-      <c r="E23" s="14"/>
-      <c r="F23" s="17"/>
-      <c r="G23" s="17"/>
-      <c r="H23" s="17"/>
-      <c r="I23" s="17"/>
-      <c r="J23" s="17"/>
+      <c r="B23" s="10"/>
+      <c r="C23" s="7"/>
+      <c r="D23" s="7"/>
+      <c r="E23" s="7"/>
+      <c r="F23" s="10"/>
+      <c r="G23" s="10"/>
+      <c r="H23" s="10"/>
+      <c r="I23" s="10"/>
+      <c r="J23" s="10"/>
     </row>
     <row r="24" spans="1:10">
       <c r="A24" s="1"/>
-      <c r="B24" s="2"/>
-      <c r="C24" s="2"/>
-      <c r="D24" s="3"/>
-      <c r="E24" s="3"/>
-      <c r="F24" s="3"/>
-      <c r="G24" s="3"/>
-      <c r="H24" s="3"/>
-      <c r="I24" s="3"/>
-      <c r="J24" s="3"/>
+      <c r="B24" s="13"/>
+      <c r="C24" s="13"/>
+      <c r="D24" s="14"/>
+      <c r="E24" s="14"/>
+      <c r="F24" s="14"/>
+      <c r="G24" s="14"/>
+      <c r="H24" s="14"/>
+      <c r="I24" s="14"/>
+      <c r="J24" s="14"/>
     </row>
     <row r="25" spans="1:10">
       <c r="A25" s="1"/>
-      <c r="B25" s="2"/>
-      <c r="C25" s="2"/>
-      <c r="D25" s="3"/>
-      <c r="E25" s="3"/>
-      <c r="F25" s="3"/>
-      <c r="G25" s="3"/>
-      <c r="H25" s="3"/>
-      <c r="I25" s="3"/>
-      <c r="J25" s="3"/>
+      <c r="B25" s="13"/>
+      <c r="C25" s="13"/>
+      <c r="D25" s="14"/>
+      <c r="E25" s="14"/>
+      <c r="F25" s="14"/>
+      <c r="G25" s="14"/>
+      <c r="H25" s="14"/>
+      <c r="I25" s="14"/>
+      <c r="J25" s="14"/>
     </row>
   </sheetData>
   <mergeCells count="9">
@@ -1461,413 +1468,411 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{37B53857-54FF-4641-AA4A-33CF3BA31AAD}">
   <dimension ref="A2:J25"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+    <sheetView topLeftCell="F1" workbookViewId="0">
+      <selection activeCell="J9" sqref="J9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16.899999999999999"/>
+  <sheetFormatPr defaultRowHeight="17.399999999999999"/>
   <cols>
-    <col min="1" max="1" width="13.1875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.25" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15.3125" customWidth="1"/>
-    <col min="4" max="4" width="15.25" customWidth="1"/>
+    <col min="1" max="1" width="13.19921875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.19921875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.296875" customWidth="1"/>
+    <col min="4" max="4" width="15.19921875" customWidth="1"/>
     <col min="5" max="5" width="11" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="9.4375" customWidth="1"/>
-    <col min="7" max="7" width="6.875" customWidth="1"/>
-    <col min="8" max="8" width="6.125" customWidth="1"/>
-    <col min="9" max="9" width="5.8125" customWidth="1"/>
-    <col min="10" max="10" width="9.8125" customWidth="1"/>
+    <col min="6" max="6" width="9.3984375" customWidth="1"/>
+    <col min="7" max="7" width="6.8984375" customWidth="1"/>
+    <col min="8" max="8" width="6.09765625" customWidth="1"/>
+    <col min="9" max="9" width="5.796875" customWidth="1"/>
+    <col min="10" max="10" width="9.796875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="1:10">
       <c r="A2" s="1"/>
-      <c r="B2" s="4" t="s">
+      <c r="B2" s="15" t="s">
         <v>36</v>
       </c>
-      <c r="C2" s="5"/>
-      <c r="D2" s="6" t="s">
+      <c r="C2" s="16"/>
+      <c r="D2" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="E2" s="4" t="s">
+      <c r="E2" s="15" t="s">
         <v>37</v>
       </c>
-      <c r="F2" s="5"/>
-      <c r="G2" s="7" t="s">
+      <c r="F2" s="16"/>
+      <c r="G2" s="17" t="s">
         <v>26</v>
       </c>
-      <c r="H2" s="8"/>
-      <c r="I2" s="8"/>
-      <c r="J2" s="9"/>
+      <c r="H2" s="18"/>
+      <c r="I2" s="18"/>
+      <c r="J2" s="19"/>
     </row>
     <row r="3" spans="1:10">
       <c r="A3" s="1"/>
-      <c r="B3" s="4" t="s">
+      <c r="B3" s="15" t="s">
         <v>6</v>
       </c>
-      <c r="C3" s="5"/>
-      <c r="D3" s="8" t="s">
+      <c r="C3" s="16"/>
+      <c r="D3" s="18" t="s">
         <v>41</v>
       </c>
-      <c r="E3" s="8"/>
-      <c r="F3" s="8"/>
-      <c r="G3" s="8"/>
-      <c r="H3" s="8"/>
-      <c r="I3" s="8"/>
-      <c r="J3" s="9"/>
-    </row>
-    <row r="4" spans="1:10" ht="17.25" thickBot="1">
+      <c r="E3" s="18"/>
+      <c r="F3" s="18"/>
+      <c r="G3" s="18"/>
+      <c r="H3" s="18"/>
+      <c r="I3" s="18"/>
+      <c r="J3" s="19"/>
+    </row>
+    <row r="4" spans="1:10" ht="18" thickBot="1">
       <c r="A4" s="1"/>
-      <c r="B4" s="10" t="s">
+      <c r="B4" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="C4" s="11" t="s">
+      <c r="C4" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="D4" s="12" t="s">
+      <c r="D4" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="E4" s="10" t="s">
+      <c r="E4" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="F4" s="10" t="s">
+      <c r="F4" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="G4" s="10" t="s">
+      <c r="G4" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="H4" s="10" t="s">
+      <c r="H4" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="I4" s="10" t="s">
+      <c r="I4" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="J4" s="10" t="s">
+      <c r="J4" s="3" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="5" spans="1:10">
       <c r="A5" s="1"/>
-      <c r="B5" s="13">
+      <c r="B5" s="6">
         <v>1</v>
       </c>
-      <c r="C5" s="14" t="s">
+      <c r="C5" s="7" t="s">
         <v>27</v>
       </c>
-      <c r="D5" s="15" t="s">
+      <c r="D5" s="8" t="s">
         <v>34</v>
       </c>
-      <c r="E5" s="16" t="s">
+      <c r="E5" s="9" t="s">
         <v>35</v>
       </c>
-      <c r="F5" s="13">
-        <v>15</v>
-      </c>
-      <c r="G5" s="13" t="s">
+      <c r="F5" s="6"/>
+      <c r="G5" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="H5" s="13" t="s">
+      <c r="H5" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="I5" s="13"/>
-      <c r="J5" s="13" t="s">
+      <c r="I5" s="6"/>
+      <c r="J5" s="6" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="6" spans="1:10">
       <c r="A6" s="1"/>
-      <c r="B6" s="13">
+      <c r="B6" s="6">
         <v>2</v>
       </c>
-      <c r="C6" s="14" t="s">
+      <c r="C6" s="7" t="s">
         <v>32</v>
       </c>
-      <c r="D6" s="15" t="s">
+      <c r="D6" s="8" t="s">
         <v>33</v>
       </c>
-      <c r="E6" s="16" t="s">
+      <c r="E6" s="9" t="s">
         <v>19</v>
       </c>
-      <c r="F6" s="13">
+      <c r="F6" s="6">
         <v>15</v>
       </c>
-      <c r="G6" s="13" t="s">
+      <c r="G6" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="H6" s="13"/>
-      <c r="I6" s="17"/>
-      <c r="J6" s="13" t="s">
+      <c r="H6" s="6"/>
+      <c r="I6" s="10"/>
+      <c r="J6" s="6" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="7" spans="1:10">
       <c r="A7" s="1"/>
-      <c r="B7" s="13">
+      <c r="B7" s="6">
         <v>3</v>
       </c>
-      <c r="C7" s="14" t="s">
+      <c r="C7" s="7" t="s">
         <v>39</v>
       </c>
-      <c r="D7" s="15" t="s">
+      <c r="D7" s="8" t="s">
         <v>40</v>
       </c>
-      <c r="E7" s="16" t="s">
+      <c r="E7" s="9" t="s">
         <v>19</v>
       </c>
-      <c r="F7" s="17">
+      <c r="F7" s="10">
         <v>7</v>
       </c>
-      <c r="G7" s="13" t="s">
+      <c r="G7" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="H7" s="13"/>
-      <c r="I7" s="17"/>
-      <c r="J7" s="13" t="s">
+      <c r="H7" s="6"/>
+      <c r="I7" s="10"/>
+      <c r="J7" s="6" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="8" spans="1:10">
       <c r="A8" s="1"/>
-      <c r="B8" s="13">
+      <c r="B8" s="6">
         <v>4</v>
       </c>
-      <c r="C8" s="14" t="s">
-        <v>65</v>
-      </c>
-      <c r="D8" s="15" t="s">
+      <c r="C8" s="7" t="s">
+        <v>64</v>
+      </c>
+      <c r="D8" s="8" t="s">
         <v>46</v>
       </c>
-      <c r="E8" s="14" t="s">
+      <c r="E8" s="7" t="s">
         <v>35</v>
       </c>
-      <c r="F8" s="17"/>
-      <c r="G8" s="13" t="s">
+      <c r="F8" s="10"/>
+      <c r="G8" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="H8" s="13"/>
-      <c r="I8" s="17"/>
-      <c r="J8" s="13" t="s">
+      <c r="H8" s="6"/>
+      <c r="I8" s="10"/>
+      <c r="J8" s="6" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="9" spans="1:10">
       <c r="A9" s="1"/>
-      <c r="B9" s="13">
+      <c r="B9" s="6">
         <v>5</v>
       </c>
-      <c r="C9" s="14" t="s">
-        <v>68</v>
-      </c>
-      <c r="D9" s="15" t="s">
-        <v>63</v>
-      </c>
-      <c r="E9" s="14" t="s">
+      <c r="C9" s="7" t="s">
+        <v>67</v>
+      </c>
+      <c r="D9" s="8" t="s">
+        <v>62</v>
+      </c>
+      <c r="E9" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="F9" s="17"/>
-      <c r="G9" s="13" t="s">
-        <v>16</v>
-      </c>
-      <c r="H9" s="17"/>
-      <c r="I9" s="17"/>
-      <c r="J9" s="13" t="s">
-        <v>18</v>
+      <c r="F9" s="10"/>
+      <c r="G9" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="H9" s="10"/>
+      <c r="I9" s="10"/>
+      <c r="J9" s="6" t="s">
+        <v>74</v>
       </c>
     </row>
     <row r="10" spans="1:10">
       <c r="A10" s="1"/>
-      <c r="B10" s="13">
+      <c r="B10" s="6">
         <v>6</v>
       </c>
-      <c r="C10" s="14"/>
-      <c r="D10" s="15"/>
-      <c r="E10" s="14"/>
-      <c r="F10" s="17"/>
-      <c r="G10" s="13"/>
-      <c r="H10" s="17"/>
-      <c r="I10" s="17"/>
-      <c r="J10" s="18"/>
+      <c r="C10" s="7"/>
+      <c r="D10" s="8"/>
+      <c r="E10" s="7"/>
+      <c r="F10" s="10"/>
+      <c r="G10" s="6"/>
+      <c r="H10" s="10"/>
+      <c r="I10" s="10"/>
+      <c r="J10" s="11"/>
     </row>
     <row r="11" spans="1:10">
       <c r="A11" s="1"/>
-      <c r="B11" s="13">
+      <c r="B11" s="6">
         <v>7</v>
       </c>
-      <c r="C11" s="14"/>
-      <c r="D11" s="15"/>
-      <c r="E11" s="14"/>
-      <c r="F11" s="17"/>
-      <c r="G11" s="13"/>
-      <c r="H11" s="17"/>
-      <c r="I11" s="17"/>
-      <c r="J11" s="13"/>
+      <c r="C11" s="7"/>
+      <c r="D11" s="8"/>
+      <c r="E11" s="7"/>
+      <c r="F11" s="10"/>
+      <c r="G11" s="6"/>
+      <c r="H11" s="10"/>
+      <c r="I11" s="10"/>
+      <c r="J11" s="6"/>
     </row>
     <row r="12" spans="1:10">
       <c r="A12" s="1"/>
-      <c r="B12" s="13"/>
-      <c r="C12" s="14"/>
-      <c r="D12" s="14"/>
-      <c r="E12" s="14"/>
-      <c r="F12" s="17"/>
-      <c r="G12" s="13"/>
-      <c r="H12" s="17"/>
-      <c r="I12" s="17"/>
-      <c r="J12" s="17"/>
+      <c r="B12" s="6"/>
+      <c r="C12" s="7"/>
+      <c r="D12" s="7"/>
+      <c r="E12" s="7"/>
+      <c r="F12" s="10"/>
+      <c r="G12" s="6"/>
+      <c r="H12" s="10"/>
+      <c r="I12" s="10"/>
+      <c r="J12" s="10"/>
     </row>
     <row r="13" spans="1:10">
       <c r="A13" s="1"/>
-      <c r="B13" s="13"/>
-      <c r="C13" s="14"/>
-      <c r="D13" s="14"/>
-      <c r="E13" s="14"/>
-      <c r="F13" s="17"/>
-      <c r="G13" s="13"/>
-      <c r="H13" s="17"/>
-      <c r="I13" s="17"/>
-      <c r="J13" s="17"/>
+      <c r="B13" s="6"/>
+      <c r="C13" s="7"/>
+      <c r="D13" s="7"/>
+      <c r="E13" s="7"/>
+      <c r="F13" s="10"/>
+      <c r="G13" s="6"/>
+      <c r="H13" s="10"/>
+      <c r="I13" s="10"/>
+      <c r="J13" s="10"/>
     </row>
     <row r="14" spans="1:10">
       <c r="A14" s="1"/>
-      <c r="B14" s="13"/>
-      <c r="C14" s="14"/>
-      <c r="D14" s="14"/>
-      <c r="E14" s="14"/>
-      <c r="F14" s="17"/>
-      <c r="G14" s="13"/>
-      <c r="H14" s="17"/>
-      <c r="I14" s="17"/>
-      <c r="J14" s="17"/>
+      <c r="B14" s="6"/>
+      <c r="C14" s="7"/>
+      <c r="D14" s="7"/>
+      <c r="E14" s="7"/>
+      <c r="F14" s="10"/>
+      <c r="G14" s="6"/>
+      <c r="H14" s="10"/>
+      <c r="I14" s="10"/>
+      <c r="J14" s="10"/>
     </row>
     <row r="15" spans="1:10">
       <c r="A15" s="1"/>
-      <c r="B15" s="13"/>
-      <c r="C15" s="14"/>
-      <c r="D15" s="14"/>
-      <c r="E15" s="14"/>
-      <c r="F15" s="17"/>
-      <c r="G15" s="13"/>
-      <c r="H15" s="17"/>
-      <c r="I15" s="17"/>
-      <c r="J15" s="17"/>
+      <c r="B15" s="6"/>
+      <c r="C15" s="7"/>
+      <c r="D15" s="7"/>
+      <c r="E15" s="7"/>
+      <c r="F15" s="10"/>
+      <c r="G15" s="6"/>
+      <c r="H15" s="10"/>
+      <c r="I15" s="10"/>
+      <c r="J15" s="10"/>
     </row>
     <row r="16" spans="1:10">
       <c r="A16" s="1"/>
-      <c r="B16" s="13"/>
-      <c r="C16" s="14"/>
-      <c r="D16" s="14"/>
-      <c r="E16" s="14"/>
-      <c r="F16" s="17"/>
-      <c r="G16" s="13"/>
-      <c r="H16" s="17"/>
-      <c r="I16" s="17"/>
-      <c r="J16" s="17"/>
+      <c r="B16" s="6"/>
+      <c r="C16" s="7"/>
+      <c r="D16" s="7"/>
+      <c r="E16" s="7"/>
+      <c r="F16" s="10"/>
+      <c r="G16" s="6"/>
+      <c r="H16" s="10"/>
+      <c r="I16" s="10"/>
+      <c r="J16" s="10"/>
     </row>
     <row r="17" spans="1:10">
       <c r="A17" s="1"/>
-      <c r="B17" s="13"/>
-      <c r="C17" s="14"/>
-      <c r="D17" s="14"/>
-      <c r="E17" s="14"/>
-      <c r="F17" s="17"/>
-      <c r="G17" s="13"/>
-      <c r="H17" s="17"/>
-      <c r="I17" s="17"/>
-      <c r="J17" s="17"/>
+      <c r="B17" s="6"/>
+      <c r="C17" s="7"/>
+      <c r="D17" s="7"/>
+      <c r="E17" s="7"/>
+      <c r="F17" s="10"/>
+      <c r="G17" s="6"/>
+      <c r="H17" s="10"/>
+      <c r="I17" s="10"/>
+      <c r="J17" s="10"/>
     </row>
     <row r="18" spans="1:10">
       <c r="A18" s="1"/>
-      <c r="B18" s="13"/>
-      <c r="C18" s="14"/>
-      <c r="D18" s="14"/>
-      <c r="E18" s="14"/>
-      <c r="F18" s="17"/>
-      <c r="G18" s="13"/>
-      <c r="H18" s="17"/>
-      <c r="I18" s="17"/>
-      <c r="J18" s="17"/>
+      <c r="B18" s="6"/>
+      <c r="C18" s="7"/>
+      <c r="D18" s="7"/>
+      <c r="E18" s="7"/>
+      <c r="F18" s="10"/>
+      <c r="G18" s="6"/>
+      <c r="H18" s="10"/>
+      <c r="I18" s="10"/>
+      <c r="J18" s="10"/>
     </row>
     <row r="19" spans="1:10">
       <c r="A19" s="1"/>
-      <c r="B19" s="13"/>
-      <c r="C19" s="14"/>
-      <c r="D19" s="14"/>
-      <c r="E19" s="14"/>
-      <c r="F19" s="17"/>
-      <c r="G19" s="13"/>
-      <c r="H19" s="17"/>
-      <c r="I19" s="17"/>
-      <c r="J19" s="17"/>
+      <c r="B19" s="6"/>
+      <c r="C19" s="7"/>
+      <c r="D19" s="7"/>
+      <c r="E19" s="7"/>
+      <c r="F19" s="10"/>
+      <c r="G19" s="6"/>
+      <c r="H19" s="10"/>
+      <c r="I19" s="10"/>
+      <c r="J19" s="10"/>
     </row>
     <row r="20" spans="1:10">
       <c r="A20" s="1"/>
-      <c r="B20" s="13"/>
-      <c r="C20" s="14"/>
-      <c r="D20" s="14"/>
-      <c r="E20" s="14"/>
-      <c r="F20" s="17"/>
-      <c r="G20" s="13"/>
-      <c r="H20" s="17"/>
-      <c r="I20" s="17"/>
-      <c r="J20" s="17"/>
+      <c r="B20" s="6"/>
+      <c r="C20" s="7"/>
+      <c r="D20" s="7"/>
+      <c r="E20" s="7"/>
+      <c r="F20" s="10"/>
+      <c r="G20" s="6"/>
+      <c r="H20" s="10"/>
+      <c r="I20" s="10"/>
+      <c r="J20" s="10"/>
     </row>
     <row r="21" spans="1:10">
       <c r="A21" s="1"/>
-      <c r="B21" s="13"/>
-      <c r="C21" s="14"/>
-      <c r="D21" s="14"/>
-      <c r="E21" s="14"/>
-      <c r="F21" s="17"/>
-      <c r="G21" s="13"/>
-      <c r="H21" s="17"/>
-      <c r="I21" s="17"/>
-      <c r="J21" s="17"/>
+      <c r="B21" s="6"/>
+      <c r="C21" s="7"/>
+      <c r="D21" s="7"/>
+      <c r="E21" s="7"/>
+      <c r="F21" s="10"/>
+      <c r="G21" s="6"/>
+      <c r="H21" s="10"/>
+      <c r="I21" s="10"/>
+      <c r="J21" s="10"/>
     </row>
     <row r="22" spans="1:10">
       <c r="A22" s="1"/>
-      <c r="B22" s="13"/>
-      <c r="C22" s="14"/>
-      <c r="D22" s="14"/>
-      <c r="E22" s="14"/>
-      <c r="F22" s="17"/>
-      <c r="G22" s="13"/>
-      <c r="H22" s="17"/>
-      <c r="I22" s="17"/>
-      <c r="J22" s="17"/>
+      <c r="B22" s="6"/>
+      <c r="C22" s="7"/>
+      <c r="D22" s="7"/>
+      <c r="E22" s="7"/>
+      <c r="F22" s="10"/>
+      <c r="G22" s="6"/>
+      <c r="H22" s="10"/>
+      <c r="I22" s="10"/>
+      <c r="J22" s="10"/>
     </row>
     <row r="23" spans="1:10">
       <c r="A23" s="1"/>
-      <c r="B23" s="17"/>
-      <c r="C23" s="14"/>
-      <c r="D23" s="14"/>
-      <c r="E23" s="14"/>
-      <c r="F23" s="17"/>
-      <c r="G23" s="17"/>
-      <c r="H23" s="17"/>
-      <c r="I23" s="17"/>
-      <c r="J23" s="17"/>
+      <c r="B23" s="10"/>
+      <c r="C23" s="7"/>
+      <c r="D23" s="7"/>
+      <c r="E23" s="7"/>
+      <c r="F23" s="10"/>
+      <c r="G23" s="10"/>
+      <c r="H23" s="10"/>
+      <c r="I23" s="10"/>
+      <c r="J23" s="10"/>
     </row>
     <row r="24" spans="1:10">
       <c r="A24" s="1"/>
-      <c r="B24" s="2"/>
-      <c r="C24" s="2"/>
-      <c r="D24" s="3"/>
-      <c r="E24" s="3"/>
-      <c r="F24" s="3"/>
-      <c r="G24" s="3"/>
-      <c r="H24" s="3"/>
-      <c r="I24" s="3"/>
-      <c r="J24" s="3"/>
+      <c r="B24" s="13"/>
+      <c r="C24" s="13"/>
+      <c r="D24" s="14"/>
+      <c r="E24" s="14"/>
+      <c r="F24" s="14"/>
+      <c r="G24" s="14"/>
+      <c r="H24" s="14"/>
+      <c r="I24" s="14"/>
+      <c r="J24" s="14"/>
     </row>
     <row r="25" spans="1:10">
       <c r="A25" s="1"/>
-      <c r="B25" s="2"/>
-      <c r="C25" s="2"/>
-      <c r="D25" s="3"/>
-      <c r="E25" s="3"/>
-      <c r="F25" s="3"/>
-      <c r="G25" s="3"/>
-      <c r="H25" s="3"/>
-      <c r="I25" s="3"/>
-      <c r="J25" s="3"/>
+      <c r="B25" s="13"/>
+      <c r="C25" s="13"/>
+      <c r="D25" s="14"/>
+      <c r="E25" s="14"/>
+      <c r="F25" s="14"/>
+      <c r="G25" s="14"/>
+      <c r="H25" s="14"/>
+      <c r="I25" s="14"/>
+      <c r="J25" s="14"/>
     </row>
   </sheetData>
   <mergeCells count="9">
@@ -1891,457 +1896,451 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0B74128D-9708-4080-AEBF-BCE94739D0EC}">
   <dimension ref="A2:J25"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F29" sqref="F29"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16.899999999999999"/>
+  <sheetFormatPr defaultRowHeight="17.399999999999999"/>
   <cols>
-    <col min="1" max="1" width="13.1875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.25" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15.3125" customWidth="1"/>
-    <col min="4" max="4" width="15.25" customWidth="1"/>
+    <col min="1" max="1" width="13.19921875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.19921875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.296875" customWidth="1"/>
+    <col min="4" max="4" width="15.19921875" customWidth="1"/>
     <col min="5" max="5" width="11" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="9.4375" customWidth="1"/>
-    <col min="7" max="7" width="6.875" customWidth="1"/>
-    <col min="8" max="8" width="6.125" customWidth="1"/>
-    <col min="9" max="9" width="12.4375" customWidth="1"/>
-    <col min="10" max="10" width="9.8125" customWidth="1"/>
+    <col min="6" max="6" width="9.3984375" customWidth="1"/>
+    <col min="7" max="7" width="6.8984375" customWidth="1"/>
+    <col min="8" max="8" width="6.09765625" customWidth="1"/>
+    <col min="9" max="9" width="12.3984375" customWidth="1"/>
+    <col min="10" max="10" width="9.796875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="1:10">
       <c r="A2" s="1"/>
-      <c r="B2" s="4" t="s">
+      <c r="B2" s="15" t="s">
         <v>36</v>
       </c>
-      <c r="C2" s="5"/>
-      <c r="D2" s="6" t="s">
-        <v>51</v>
-      </c>
-      <c r="E2" s="4" t="s">
+      <c r="C2" s="16"/>
+      <c r="D2" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="E2" s="15" t="s">
         <v>37</v>
       </c>
-      <c r="F2" s="5"/>
-      <c r="G2" s="7" t="s">
+      <c r="F2" s="16"/>
+      <c r="G2" s="17" t="s">
         <v>49</v>
       </c>
-      <c r="H2" s="8"/>
-      <c r="I2" s="8"/>
-      <c r="J2" s="9"/>
+      <c r="H2" s="18"/>
+      <c r="I2" s="18"/>
+      <c r="J2" s="19"/>
     </row>
     <row r="3" spans="1:10">
       <c r="A3" s="1"/>
-      <c r="B3" s="4" t="s">
+      <c r="B3" s="15" t="s">
         <v>6</v>
       </c>
-      <c r="C3" s="5"/>
-      <c r="D3" s="8" t="s">
-        <v>52</v>
-      </c>
-      <c r="E3" s="8"/>
-      <c r="F3" s="8"/>
-      <c r="G3" s="8"/>
-      <c r="H3" s="8"/>
-      <c r="I3" s="8"/>
-      <c r="J3" s="9"/>
-    </row>
-    <row r="4" spans="1:10" ht="17.25" thickBot="1">
+      <c r="C3" s="16"/>
+      <c r="D3" s="18" t="s">
+        <v>51</v>
+      </c>
+      <c r="E3" s="18"/>
+      <c r="F3" s="18"/>
+      <c r="G3" s="18"/>
+      <c r="H3" s="18"/>
+      <c r="I3" s="18"/>
+      <c r="J3" s="19"/>
+    </row>
+    <row r="4" spans="1:10" ht="18" thickBot="1">
       <c r="A4" s="1"/>
-      <c r="B4" s="10" t="s">
+      <c r="B4" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="C4" s="11" t="s">
+      <c r="C4" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="D4" s="12" t="s">
+      <c r="D4" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="E4" s="10" t="s">
+      <c r="E4" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="F4" s="10" t="s">
+      <c r="F4" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="G4" s="10" t="s">
+      <c r="G4" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="H4" s="10" t="s">
+      <c r="H4" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="I4" s="10" t="s">
+      <c r="I4" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="J4" s="10" t="s">
+      <c r="J4" s="3" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="5" spans="1:10" ht="16.899999999999999" customHeight="1">
+    <row r="5" spans="1:10" ht="16.95" customHeight="1">
       <c r="A5" s="1"/>
-      <c r="B5" s="13">
+      <c r="B5" s="6">
         <v>1</v>
       </c>
-      <c r="C5" s="14" t="s">
+      <c r="C5" s="7" t="s">
         <v>27</v>
       </c>
-      <c r="D5" s="15" t="s">
-        <v>54</v>
-      </c>
-      <c r="E5" s="16" t="s">
+      <c r="D5" s="8" t="s">
+        <v>53</v>
+      </c>
+      <c r="E5" s="9" t="s">
         <v>35</v>
       </c>
-      <c r="F5" s="13">
-        <v>15</v>
-      </c>
-      <c r="G5" s="13" t="s">
+      <c r="F5" s="6"/>
+      <c r="G5" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="H5" s="13"/>
-      <c r="I5" s="13" t="s">
+      <c r="H5" s="6"/>
+      <c r="I5" s="6" t="s">
         <v>44</v>
       </c>
-      <c r="J5" s="13" t="s">
+      <c r="J5" s="6" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="6" spans="1:10">
       <c r="A6" s="1"/>
-      <c r="B6" s="13">
+      <c r="B6" s="6">
         <v>2</v>
       </c>
-      <c r="C6" s="14" t="s">
+      <c r="C6" s="7" t="s">
         <v>28</v>
       </c>
-      <c r="D6" s="15" t="s">
+      <c r="D6" s="8" t="s">
         <v>29</v>
       </c>
-      <c r="E6" s="16" t="s">
+      <c r="E6" s="9" t="s">
         <v>19</v>
       </c>
-      <c r="F6" s="13">
+      <c r="F6" s="6">
         <v>15</v>
       </c>
-      <c r="G6" s="13" t="s">
+      <c r="G6" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="H6" s="19"/>
-      <c r="I6" s="13" t="s">
+      <c r="H6" s="12"/>
+      <c r="I6" s="6" t="s">
         <v>45</v>
       </c>
-      <c r="J6" s="13" t="s">
+      <c r="J6" s="6" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="7" spans="1:10">
       <c r="A7" s="1"/>
-      <c r="B7" s="13">
+      <c r="B7" s="6">
         <v>3</v>
       </c>
-      <c r="C7" s="14" t="s">
+      <c r="C7" s="7" t="s">
         <v>50</v>
       </c>
-      <c r="D7" s="15" t="s">
-        <v>53</v>
-      </c>
-      <c r="E7" s="16" t="s">
+      <c r="D7" s="8" t="s">
+        <v>52</v>
+      </c>
+      <c r="E7" s="9" t="s">
         <v>35</v>
       </c>
-      <c r="F7" s="17">
-        <v>10</v>
-      </c>
-      <c r="G7" s="13" t="s">
+      <c r="F7" s="10"/>
+      <c r="G7" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="H7" s="13" t="s">
+      <c r="H7" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="I7" s="17"/>
-      <c r="J7" s="13" t="s">
+      <c r="I7" s="10"/>
+      <c r="J7" s="6" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="8" spans="1:10">
       <c r="A8" s="1"/>
-      <c r="B8" s="13">
+      <c r="B8" s="6">
         <v>4</v>
       </c>
-      <c r="C8" s="14" t="s">
+      <c r="C8" s="7" t="s">
         <v>43</v>
       </c>
-      <c r="D8" s="15" t="s">
-        <v>58</v>
-      </c>
-      <c r="E8" s="16" t="s">
+      <c r="D8" s="8" t="s">
+        <v>57</v>
+      </c>
+      <c r="E8" s="9" t="s">
         <v>35</v>
       </c>
-      <c r="F8" s="17">
-        <v>3</v>
-      </c>
-      <c r="G8" s="13" t="s">
+      <c r="F8" s="10"/>
+      <c r="G8" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="H8" s="13"/>
-      <c r="I8" s="17"/>
-      <c r="J8" s="13" t="s">
+      <c r="H8" s="6"/>
+      <c r="I8" s="10"/>
+      <c r="J8" s="6" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="9" spans="1:10">
       <c r="A9" s="1"/>
-      <c r="B9" s="13">
+      <c r="B9" s="6">
         <v>5</v>
       </c>
-      <c r="C9" s="14" t="s">
-        <v>57</v>
-      </c>
-      <c r="D9" s="15" t="s">
+      <c r="C9" s="7" t="s">
+        <v>56</v>
+      </c>
+      <c r="D9" s="8" t="s">
         <v>48</v>
       </c>
-      <c r="E9" s="14" t="s">
-        <v>55</v>
-      </c>
-      <c r="F9" s="17"/>
-      <c r="G9" s="13" t="s">
+      <c r="E9" s="7" t="s">
+        <v>54</v>
+      </c>
+      <c r="F9" s="10"/>
+      <c r="G9" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="H9" s="13"/>
-      <c r="I9" s="17"/>
-      <c r="J9" s="13" t="s">
+      <c r="H9" s="6"/>
+      <c r="I9" s="10"/>
+      <c r="J9" s="6" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="10" spans="1:10">
       <c r="A10" s="1"/>
-      <c r="B10" s="13">
+      <c r="B10" s="6">
         <v>6</v>
       </c>
-      <c r="C10" s="14" t="s">
-        <v>59</v>
-      </c>
-      <c r="D10" s="15" t="s">
-        <v>62</v>
-      </c>
-      <c r="E10" s="16" t="s">
+      <c r="C10" s="7" t="s">
+        <v>58</v>
+      </c>
+      <c r="D10" s="8" t="s">
+        <v>61</v>
+      </c>
+      <c r="E10" s="9" t="s">
         <v>35</v>
       </c>
-      <c r="F10" s="17">
-        <v>10</v>
-      </c>
-      <c r="G10" s="13" t="s">
+      <c r="F10" s="10"/>
+      <c r="G10" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="H10" s="17"/>
-      <c r="I10" s="17"/>
-      <c r="J10" s="13" t="s">
+      <c r="H10" s="10"/>
+      <c r="I10" s="10"/>
+      <c r="J10" s="6" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="11" spans="1:10">
       <c r="A11" s="1"/>
-      <c r="B11" s="13">
+      <c r="B11" s="6">
         <v>7</v>
       </c>
-      <c r="C11" s="14" t="s">
+      <c r="C11" s="7" t="s">
+        <v>59</v>
+      </c>
+      <c r="D11" s="8" t="s">
         <v>60</v>
       </c>
-      <c r="D11" s="15" t="s">
-        <v>61</v>
-      </c>
-      <c r="E11" s="16" t="s">
+      <c r="E11" s="9" t="s">
         <v>19</v>
       </c>
-      <c r="F11" s="17">
+      <c r="F11" s="10">
         <v>50</v>
       </c>
-      <c r="G11" s="13" t="s">
+      <c r="G11" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="H11" s="17"/>
-      <c r="I11" s="17"/>
-      <c r="J11" s="13" t="s">
+      <c r="H11" s="10"/>
+      <c r="I11" s="10"/>
+      <c r="J11" s="6" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="12" spans="1:10">
       <c r="A12" s="1"/>
-      <c r="B12" s="13">
+      <c r="B12" s="6">
         <v>8</v>
       </c>
-      <c r="C12" s="14" t="s">
+      <c r="C12" s="7" t="s">
+        <v>65</v>
+      </c>
+      <c r="D12" s="7" t="s">
         <v>66</v>
       </c>
-      <c r="D12" s="14" t="s">
-        <v>67</v>
-      </c>
-      <c r="E12" s="14" t="s">
+      <c r="E12" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="F12" s="17"/>
-      <c r="G12" s="13" t="s">
-        <v>16</v>
-      </c>
-      <c r="H12" s="17"/>
-      <c r="I12" s="17"/>
-      <c r="J12" s="13" t="s">
-        <v>18</v>
+      <c r="F12" s="10">
+        <v>10</v>
+      </c>
+      <c r="G12" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="H12" s="10"/>
+      <c r="I12" s="10"/>
+      <c r="J12" s="6" t="s">
+        <v>74</v>
       </c>
     </row>
     <row r="13" spans="1:10">
       <c r="A13" s="1"/>
-      <c r="B13" s="13">
+      <c r="B13" s="6">
         <v>9</v>
       </c>
-      <c r="C13" s="14"/>
-      <c r="D13" s="14"/>
-      <c r="E13" s="14"/>
-      <c r="F13" s="17"/>
-      <c r="G13" s="13"/>
-      <c r="H13" s="17"/>
-      <c r="I13" s="17"/>
-      <c r="J13" s="17"/>
+      <c r="C13" s="7"/>
+      <c r="D13" s="7"/>
+      <c r="E13" s="7"/>
+      <c r="F13" s="10"/>
+      <c r="G13" s="6"/>
+      <c r="H13" s="10"/>
+      <c r="I13" s="10"/>
+      <c r="J13" s="10"/>
     </row>
     <row r="14" spans="1:10">
       <c r="A14" s="1"/>
-      <c r="B14" s="13"/>
-      <c r="C14" s="14"/>
-      <c r="D14" s="14"/>
-      <c r="E14" s="14"/>
-      <c r="F14" s="17"/>
-      <c r="G14" s="13"/>
-      <c r="H14" s="17"/>
-      <c r="I14" s="17"/>
-      <c r="J14" s="17"/>
+      <c r="B14" s="6"/>
+      <c r="C14" s="7"/>
+      <c r="D14" s="7"/>
+      <c r="E14" s="7"/>
+      <c r="F14" s="10"/>
+      <c r="G14" s="6"/>
+      <c r="H14" s="10"/>
+      <c r="I14" s="10"/>
+      <c r="J14" s="10"/>
     </row>
     <row r="15" spans="1:10">
       <c r="A15" s="1"/>
-      <c r="B15" s="13"/>
-      <c r="C15" s="14"/>
-      <c r="D15" s="14"/>
-      <c r="E15" s="14"/>
-      <c r="F15" s="17"/>
-      <c r="G15" s="13"/>
-      <c r="H15" s="17"/>
-      <c r="I15" s="17"/>
-      <c r="J15" s="17"/>
+      <c r="B15" s="6"/>
+      <c r="C15" s="7"/>
+      <c r="D15" s="7"/>
+      <c r="E15" s="7"/>
+      <c r="F15" s="10"/>
+      <c r="G15" s="6"/>
+      <c r="H15" s="10"/>
+      <c r="I15" s="10"/>
+      <c r="J15" s="10"/>
     </row>
     <row r="16" spans="1:10">
       <c r="A16" s="1"/>
-      <c r="B16" s="13"/>
-      <c r="C16" s="14"/>
-      <c r="D16" s="14"/>
-      <c r="E16" s="14"/>
-      <c r="F16" s="17"/>
-      <c r="G16" s="13"/>
-      <c r="H16" s="17"/>
-      <c r="I16" s="17"/>
-      <c r="J16" s="17"/>
+      <c r="B16" s="6"/>
+      <c r="C16" s="7"/>
+      <c r="D16" s="7"/>
+      <c r="E16" s="7"/>
+      <c r="F16" s="10"/>
+      <c r="G16" s="6"/>
+      <c r="H16" s="10"/>
+      <c r="I16" s="10"/>
+      <c r="J16" s="10"/>
     </row>
     <row r="17" spans="1:10">
       <c r="A17" s="1"/>
-      <c r="B17" s="13"/>
-      <c r="C17" s="14"/>
-      <c r="D17" s="14"/>
-      <c r="E17" s="14"/>
-      <c r="F17" s="17"/>
-      <c r="G17" s="13"/>
-      <c r="H17" s="17"/>
-      <c r="I17" s="17"/>
-      <c r="J17" s="17"/>
+      <c r="B17" s="6"/>
+      <c r="C17" s="7"/>
+      <c r="D17" s="7"/>
+      <c r="E17" s="7"/>
+      <c r="F17" s="10"/>
+      <c r="G17" s="6"/>
+      <c r="H17" s="10"/>
+      <c r="I17" s="10"/>
+      <c r="J17" s="10"/>
     </row>
     <row r="18" spans="1:10">
       <c r="A18" s="1"/>
-      <c r="B18" s="13"/>
-      <c r="C18" s="14"/>
-      <c r="D18" s="14"/>
-      <c r="E18" s="14"/>
-      <c r="F18" s="17"/>
-      <c r="G18" s="13"/>
-      <c r="H18" s="17"/>
-      <c r="I18" s="17"/>
-      <c r="J18" s="17"/>
+      <c r="B18" s="6"/>
+      <c r="C18" s="7"/>
+      <c r="D18" s="7"/>
+      <c r="E18" s="7"/>
+      <c r="F18" s="10"/>
+      <c r="G18" s="6"/>
+      <c r="H18" s="10"/>
+      <c r="I18" s="10"/>
+      <c r="J18" s="10"/>
     </row>
     <row r="19" spans="1:10">
       <c r="A19" s="1"/>
-      <c r="B19" s="13"/>
-      <c r="C19" s="14"/>
-      <c r="D19" s="14"/>
-      <c r="E19" s="14"/>
-      <c r="F19" s="17"/>
-      <c r="G19" s="13"/>
-      <c r="H19" s="17"/>
-      <c r="I19" s="17"/>
-      <c r="J19" s="17"/>
+      <c r="B19" s="6"/>
+      <c r="C19" s="7"/>
+      <c r="D19" s="7"/>
+      <c r="E19" s="7"/>
+      <c r="F19" s="10"/>
+      <c r="G19" s="6"/>
+      <c r="H19" s="10"/>
+      <c r="I19" s="10"/>
+      <c r="J19" s="10"/>
     </row>
     <row r="20" spans="1:10">
       <c r="A20" s="1"/>
-      <c r="B20" s="13"/>
-      <c r="C20" s="14"/>
-      <c r="D20" s="14"/>
-      <c r="E20" s="14"/>
-      <c r="F20" s="17"/>
-      <c r="G20" s="13"/>
-      <c r="H20" s="17"/>
-      <c r="I20" s="17"/>
-      <c r="J20" s="17"/>
+      <c r="B20" s="6"/>
+      <c r="C20" s="7"/>
+      <c r="D20" s="7"/>
+      <c r="E20" s="7"/>
+      <c r="F20" s="10"/>
+      <c r="G20" s="6"/>
+      <c r="H20" s="10"/>
+      <c r="I20" s="10"/>
+      <c r="J20" s="10"/>
     </row>
     <row r="21" spans="1:10">
       <c r="A21" s="1"/>
-      <c r="B21" s="13"/>
-      <c r="C21" s="14"/>
-      <c r="D21" s="14"/>
-      <c r="E21" s="14"/>
-      <c r="F21" s="17"/>
-      <c r="G21" s="13"/>
-      <c r="H21" s="17"/>
-      <c r="I21" s="17"/>
-      <c r="J21" s="17"/>
+      <c r="B21" s="6"/>
+      <c r="C21" s="7"/>
+      <c r="D21" s="7"/>
+      <c r="E21" s="7"/>
+      <c r="F21" s="10"/>
+      <c r="G21" s="6"/>
+      <c r="H21" s="10"/>
+      <c r="I21" s="10"/>
+      <c r="J21" s="10"/>
     </row>
     <row r="22" spans="1:10">
       <c r="A22" s="1"/>
-      <c r="B22" s="13"/>
-      <c r="C22" s="14"/>
-      <c r="D22" s="14"/>
-      <c r="E22" s="14"/>
-      <c r="F22" s="17"/>
-      <c r="G22" s="13"/>
-      <c r="H22" s="17"/>
-      <c r="I22" s="17"/>
-      <c r="J22" s="17"/>
+      <c r="B22" s="6"/>
+      <c r="C22" s="7"/>
+      <c r="D22" s="7"/>
+      <c r="E22" s="7"/>
+      <c r="F22" s="10"/>
+      <c r="G22" s="6"/>
+      <c r="H22" s="10"/>
+      <c r="I22" s="10"/>
+      <c r="J22" s="10"/>
     </row>
     <row r="23" spans="1:10">
       <c r="A23" s="1"/>
-      <c r="B23" s="17"/>
-      <c r="C23" s="14"/>
-      <c r="D23" s="14"/>
-      <c r="E23" s="14"/>
-      <c r="F23" s="17"/>
-      <c r="G23" s="17"/>
-      <c r="H23" s="17"/>
-      <c r="I23" s="17"/>
-      <c r="J23" s="17"/>
+      <c r="B23" s="10"/>
+      <c r="C23" s="7"/>
+      <c r="D23" s="7"/>
+      <c r="E23" s="7"/>
+      <c r="F23" s="10"/>
+      <c r="G23" s="10"/>
+      <c r="H23" s="10"/>
+      <c r="I23" s="10"/>
+      <c r="J23" s="10"/>
     </row>
     <row r="24" spans="1:10">
       <c r="A24" s="1"/>
-      <c r="B24" s="2"/>
-      <c r="C24" s="2"/>
-      <c r="D24" s="3"/>
-      <c r="E24" s="3"/>
-      <c r="F24" s="3"/>
-      <c r="G24" s="3"/>
-      <c r="H24" s="3"/>
-      <c r="I24" s="3"/>
-      <c r="J24" s="3"/>
+      <c r="B24" s="13"/>
+      <c r="C24" s="13"/>
+      <c r="D24" s="14"/>
+      <c r="E24" s="14"/>
+      <c r="F24" s="14"/>
+      <c r="G24" s="14"/>
+      <c r="H24" s="14"/>
+      <c r="I24" s="14"/>
+      <c r="J24" s="14"/>
     </row>
     <row r="25" spans="1:10">
       <c r="A25" s="1"/>
-      <c r="B25" s="2"/>
-      <c r="C25" s="2"/>
-      <c r="D25" s="3"/>
-      <c r="E25" s="3"/>
-      <c r="F25" s="3"/>
-      <c r="G25" s="3"/>
-      <c r="H25" s="3"/>
-      <c r="I25" s="3"/>
-      <c r="J25" s="3"/>
+      <c r="B25" s="13"/>
+      <c r="C25" s="13"/>
+      <c r="D25" s="14"/>
+      <c r="E25" s="14"/>
+      <c r="F25" s="14"/>
+      <c r="G25" s="14"/>
+      <c r="H25" s="14"/>
+      <c r="I25" s="14"/>
+      <c r="J25" s="14"/>
     </row>
   </sheetData>
   <mergeCells count="9">

</xml_diff>